<commit_message>
Updating repo with latestCodes
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Sno</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Accepts no parameters and waits for page to render itself. It does that by observing network state. Step never triggers test failure and waits for maximum period of 30 seconds</t>
+  </si>
+  <si>
+    <t>textBoxShouldHaveValue</t>
+  </si>
+  <si>
+    <t>Accepts two parameters @locator and @testData. It gets the text from textBox and validates against the @testData provided. If the validation fails testing should still continue</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,12 +739,26 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added tests For Become Partner Page
1. Add test Cases for Become partner page
2. Fix issues with String matching for element text
3. Add Methods to check if button is enabled or disabled
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Sno</t>
   </si>
@@ -143,6 +143,27 @@
   </si>
   <si>
     <t>Accepts two parameters @locator and @testData. It gets the text from textBox and validates against the @testData provided. If the validation fails testing should still continue</t>
+  </si>
+  <si>
+    <t>elementShouldNotBePresent</t>
+  </si>
+  <si>
+    <t>Accepts no parameters and verifies element is not available in DOM. Returns true if element is not available in DOM</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>isButtonEnabled</t>
+  </si>
+  <si>
+    <t>isButtonDisabled</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Checks if the Button is enabled. Returns true if the button is enabled</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Checks if the Button is disabled Returns true if the button is disabled</t>
   </si>
 </sst>
 </file>
@@ -186,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -195,6 +216,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -762,6 +785,48 @@
         <v>40</v>
       </c>
     </row>
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B2:D16">
     <sortCondition ref="B2"/>

</xml_diff>

<commit_message>
added tests for downloads page
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/CompilerDictionary/KeywordDictionary/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4640E36-0BB5-D345-AD65-EC2F268E7F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="19140" windowHeight="7090"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
@@ -169,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,7 +223,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,14 +233,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -273,7 +281,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -345,7 +353,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,22 +526,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="34.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -547,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -561,7 +569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -575,7 +583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -589,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -603,7 +611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -617,7 +625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -631,7 +639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -645,7 +653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -659,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -673,7 +681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -687,7 +695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -701,7 +709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -715,7 +723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -729,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -743,7 +751,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -757,7 +765,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -771,7 +779,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -785,7 +793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -799,11 +807,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
       <c r="C20" t="s">
@@ -813,11 +821,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
       <c r="C21" t="s">
@@ -828,7 +836,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D16">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add functionality to detect warning Sign on input fields
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Sno</t>
   </si>
@@ -164,6 +164,21 @@
   </si>
   <si>
     <t>Accepts one parameter @locator. Checks if the Button is disabled Returns true if the button is disabled</t>
+  </si>
+  <si>
+    <t>verifyWarningIsDisplayedForTheField</t>
+  </si>
+  <si>
+    <t>Text Field, DropDowns</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Checks if the warning symbol is displayed for the input fields</t>
+  </si>
+  <si>
+    <t>verifyNoWarningIsDisplayedForTheField</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Verifies no warning symbol is displayed for the input fields</t>
   </si>
 </sst>
 </file>
@@ -519,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.90625" customWidth="1"/>
@@ -827,6 +842,34 @@
         <v>49</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B2:D16">
     <sortCondition ref="B2"/>

</xml_diff>

<commit_message>
update locators for testing
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/CompilerDictionary/KeywordDictionary/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4640E36-0BB5-D345-AD65-EC2F268E7F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="140" windowWidth="19140" windowHeight="7090"/>
   </bookViews>
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Sno</t>
   </si>
@@ -170,12 +164,27 @@
   </si>
   <si>
     <t>Accepts one parameter @locator. Checks if the Button is disabled Returns true if the button is disabled</t>
+  </si>
+  <si>
+    <t>verifyWarningIsDisplayedForTheField</t>
+  </si>
+  <si>
+    <t>Text Field, DropDowns</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Checks if the warning symbol is displayed for the input fields</t>
+  </si>
+  <si>
+    <t>verifyNoWarningIsDisplayedForTheField</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Verifies no warning symbol is displayed for the input fields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -223,6 +232,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,17 +243,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +288,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -353,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -526,22 +533,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -555,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -569,7 +576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -583,7 +590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -597,7 +604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -611,7 +618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -625,7 +632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -639,7 +646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -653,7 +660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -667,7 +674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -681,7 +688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -695,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -709,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -723,7 +730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -737,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -751,7 +758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -765,7 +772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -779,7 +786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -793,7 +800,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -807,11 +814,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C20" t="s">
@@ -821,11 +828,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C21" t="s">
@@ -835,8 +842,36 @@
         <v>49</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D16">
+  <sortState ref="B2:D16">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes done to Introduce Named Configuration for XLSX reader
1. XLSX file reads file by column names instead of position.
2. Made changes in compiler to detect incorrect parameters for the actions.
3. Made changes in Keyword library to introduce action description.
4. Made changes to make reports more comprehensive and readable.
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/CompilerDictionary/KeywordDictionary/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9DCF9E-94FD-7548-91A2-25D5ACC61816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="19140" windowHeight="7090"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Sno</t>
   </si>
@@ -148,9 +154,6 @@
     <t>elementShouldNotBePresent</t>
   </si>
   <si>
-    <t>Accepts no parameters and verifies element is not available in DOM. Returns true if element is not available in DOM</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -179,12 +182,84 @@
   </si>
   <si>
     <t>Accepts one parameter @locator. Verifies no warning symbol is displayed for the input fields</t>
+  </si>
+  <si>
+    <t>Function Description</t>
+  </si>
+  <si>
+    <t>Verify {@locator} must be visible on the page.</t>
+  </si>
+  <si>
+    <t>Click on {@locator}.</t>
+  </si>
+  <si>
+    <t>Trigger lazy load by scrolling down page a little and then click on {@locator} once it appears on page.</t>
+  </si>
+  <si>
+    <t>Wait for visibility of {@locator} and then click on it.</t>
+  </si>
+  <si>
+    <t>Select the item at index {@testData} from dropdown {@locator}.</t>
+  </si>
+  <si>
+    <t>Select the item with value {@testData} from dropdown {@locator}.</t>
+  </si>
+  <si>
+    <t>Validate that {@locator} has text equal to {@testData}.</t>
+  </si>
+  <si>
+    <t>Close the currently active browser tab or page.</t>
+  </si>
+  <si>
+    <t>Close the entire browser session.</t>
+  </si>
+  <si>
+    <t>Navigate to the URL provided in {@testData}.</t>
+  </si>
+  <si>
+    <t>Launch a browser instance as per {@testData}.</t>
+  </si>
+  <si>
+    <t>Launch a headless browser instance as per {@testData} for faster testing.</t>
+  </si>
+  <si>
+    <t>Enter {@testData} into text field identified by {@locator}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press Keyboard key {@testData}. </t>
+  </si>
+  <si>
+    <t>Wait for the page to finish rendering without causing test failure.</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator and verifies element is not available in DOM. Returns true if element is not available in DOM</t>
+  </si>
+  <si>
+    <t>Verify if button {@locator} is enabled.</t>
+  </si>
+  <si>
+    <t>Verify if button {@locator} is disabled.</t>
+  </si>
+  <si>
+    <t>Verify that a warning icon is shown for field {@locator}.</t>
+  </si>
+  <si>
+    <t>Verify that no warning icon is shown for field {@locator}.</t>
+  </si>
+  <si>
+    <t>Verify that the value of textBox {@locator} must be equal to {@testData}.</t>
+  </si>
+  <si>
+    <t>Verify that the value of textBox {@locator} should be equal to {@testData}.</t>
+  </si>
+  <si>
+    <t>Verify that the {@locator} is not present in the DOM.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,17 +297,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -243,14 +317,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -288,7 +365,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -360,7 +437,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -533,345 +610,416 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.90625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="E6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="E7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="E8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="E9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="E10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="E11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="E18" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>54</v>
+      <c r="E23" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D16">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>